<commit_message>
Initial commit of docs
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F066B4C8-57DC-4BBC-A561-CA3CF9CAE585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C22B0C5-F52A-4E2D-9803-33B4F9AFD408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,17 +633,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.69921875" customWidth="1"/>
-    <col min="2" max="2" width="17.09765625" customWidth="1"/>
-    <col min="5" max="5" width="28.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.296875" customWidth="1"/>
+    <col min="2" max="3" width="20.69921875" customWidth="1"/>
+    <col min="6" max="6" width="8.296875" customWidth="1"/>
     <col min="7" max="7" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -655,13 +658,13 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>21</v>
@@ -680,17 +683,17 @@
       <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>50</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
       <c r="F2">
-        <f>C2*D2</f>
+        <f>D2*E2</f>
         <v>4</v>
       </c>
       <c r="G2" t="s">
@@ -708,17 +711,17 @@
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.9</v>
       </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
       <c r="F3">
-        <f>C3*D3</f>
+        <f>D3*E3</f>
         <v>11.399999999999999</v>
       </c>
       <c r="G3" t="s">
@@ -732,17 +735,17 @@
       <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>1.26</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
       <c r="F4">
-        <f t="shared" ref="F4" si="0">C4*D4</f>
+        <f>D4*E4</f>
         <v>3.7800000000000002</v>
       </c>
       <c r="G4" t="s">
@@ -756,17 +759,17 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.25</v>
       </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
       <c r="F5">
-        <f>C5*D5</f>
+        <f>D5*E5</f>
         <v>0.75</v>
       </c>
       <c r="G5" t="s">
@@ -780,17 +783,17 @@
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="C6" t="s">
+        <v>43</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
       <c r="F6">
-        <f>C6*D6</f>
+        <f>D6*E6</f>
         <v>0.57999999999999996</v>
       </c>
       <c r="G6" t="s">
@@ -804,17 +807,17 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C7">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>42</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>0.7</v>
       </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
       <c r="F7">
-        <f>C7*D7</f>
+        <f>D7*E7</f>
         <v>0.7</v>
       </c>
       <c r="G7" t="s">
@@ -828,17 +831,17 @@
       <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>22</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
       <c r="F8">
-        <f>C8*D8</f>
+        <f>D8*E8</f>
         <v>1.1100000000000001</v>
       </c>
       <c r="G8" t="s">
@@ -852,17 +855,17 @@
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>58</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>2.89</v>
       </c>
-      <c r="E9" t="s">
-        <v>58</v>
-      </c>
       <c r="F9">
-        <f>C9*D9</f>
+        <f>D9*E9</f>
         <v>2.89</v>
       </c>
       <c r="G9" t="s">
@@ -876,17 +879,17 @@
       <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10">
         <v>3</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.1399999999999999</v>
       </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
       <c r="F10">
-        <f>C10*D10</f>
+        <f>D10*E10</f>
         <v>3.42</v>
       </c>
       <c r="G10" t="s">
@@ -900,17 +903,17 @@
       <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="C11">
-        <v>1</v>
+      <c r="C11" t="s">
+        <v>4</v>
       </c>
       <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>0.47</v>
       </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
       <c r="F11">
-        <f t="shared" ref="F11:F14" si="1">C11*D11</f>
+        <f>D11*E11</f>
         <v>0.47</v>
       </c>
       <c r="G11" t="s">
@@ -924,17 +927,17 @@
       <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12">
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.03</v>
       </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f>D12*E12</f>
         <v>0.15</v>
       </c>
       <c r="G12" t="s">
@@ -948,17 +951,17 @@
       <c r="B13" t="s">
         <v>64</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13">
         <v>7</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.03</v>
       </c>
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f>D13*E13</f>
         <v>0.21</v>
       </c>
       <c r="G13" t="s">
@@ -972,17 +975,17 @@
       <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
         <v>4</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.08</v>
       </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f>D14*E14</f>
         <v>0.32</v>
       </c>
       <c r="G14" t="s">
@@ -996,17 +999,17 @@
       <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.19</v>
       </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
       <c r="F15">
-        <f>C15*D15</f>
+        <f>D15*E15</f>
         <v>2.4700000000000002</v>
       </c>
       <c r="G15" t="s">
@@ -1020,17 +1023,17 @@
       <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>6</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>1.33</v>
       </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
       <c r="F16">
-        <f>C16*D16</f>
+        <f>D16*E16</f>
         <v>1.33</v>
       </c>
       <c r="G16" t="s">
@@ -1044,17 +1047,17 @@
       <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
-        <v>1</v>
+      <c r="C17" t="s">
+        <v>40</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>0.13</v>
       </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
       <c r="F17">
-        <f>C17*D17</f>
+        <f>D17*E17</f>
         <v>0.13</v>
       </c>
       <c r="G17" t="s">
@@ -1068,17 +1071,17 @@
       <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" t="s">
+        <v>81</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
         <v>0.68</v>
       </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
       <c r="F18">
-        <f t="shared" ref="F18:F23" si="2">C18*D18</f>
+        <f>D18*E18</f>
         <v>0.68</v>
       </c>
       <c r="G18" t="s">
@@ -1092,17 +1095,17 @@
       <c r="B19" t="s">
         <v>69</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="C19" t="s">
+        <v>82</v>
       </c>
       <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
         <v>0.65</v>
       </c>
-      <c r="E19" t="s">
-        <v>82</v>
-      </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f>D19*E19</f>
         <v>0.65</v>
       </c>
       <c r="G19" t="s">
@@ -1116,17 +1119,17 @@
       <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="C20">
-        <v>1</v>
+      <c r="C20" t="s">
+        <v>83</v>
       </c>
       <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>0.21</v>
       </c>
-      <c r="E20" t="s">
-        <v>83</v>
-      </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f>D20*E20</f>
         <v>0.21</v>
       </c>
     </row>
@@ -1137,17 +1140,17 @@
       <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="C21">
-        <v>1</v>
+      <c r="C21" t="s">
+        <v>84</v>
       </c>
       <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
         <v>0.24</v>
       </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f>D21*E21</f>
         <v>0.24</v>
       </c>
     </row>
@@ -1158,17 +1161,17 @@
       <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22">
         <v>10</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>0.05</v>
       </c>
-      <c r="E22" t="s">
-        <v>85</v>
-      </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f>D22*E22</f>
         <v>0.5</v>
       </c>
     </row>
@@ -1179,22 +1182,22 @@
       <c r="B23" t="s">
         <v>90</v>
       </c>
-      <c r="C23">
-        <v>1</v>
+      <c r="C23" t="s">
+        <v>91</v>
       </c>
       <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
         <v>0.33</v>
       </c>
-      <c r="E23" t="s">
-        <v>91</v>
-      </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f>D23*E23</f>
         <v>0.33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup scale="87" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3.2 initial commit, changed FETs to TO-220s
</commit_message>
<xml_diff>
--- a/board/BOM.xlsx
+++ b/board/BOM.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BDF2B2-3555-4978-B54B-A18F7669D9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC029A2-D1A1-4834-9DB4-0DA1C1A2F28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,12 +102,6 @@
     <t>K78U05-500R3</t>
   </si>
   <si>
-    <t>742-SIR5802DP-T1-RE3CT-ND</t>
-  </si>
-  <si>
-    <t>SIR5802DP-T1-RE3</t>
-  </si>
-  <si>
     <t>DGD2304S8-13DICT-ND</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>C9</t>
+  </si>
+  <si>
+    <t>IRFB7730PBF-ND</t>
+  </si>
+  <si>
+    <t>IRFB7730PBF</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,18 +685,18 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -709,32 +709,32 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H2">
         <f>SUM(F1:F91)</f>
-        <v>35.119999999999997</v>
+        <v>43.219999999999992</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
       <c r="E3">
-        <v>1.9</v>
+        <v>3.25</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>11.399999999999999</v>
+        <v>19.5</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -742,10 +742,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -761,18 +761,18 @@
         <v>3.7800000000000002</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -785,18 +785,18 @@
         <v>0.75</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -809,18 +809,18 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -833,15 +833,15 @@
         <v>0.7</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -857,7 +857,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -868,7 +868,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -881,18 +881,18 @@
         <v>2.89</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -905,15 +905,15 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -934,13 +934,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -953,18 +953,18 @@
         <v>0.15</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -977,18 +977,18 @@
         <v>0.21</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -1001,18 +1001,18 @@
         <v>0.18</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1025,18 +1025,18 @@
         <v>0.08</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>13</v>
@@ -1049,7 +1049,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1057,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1073,18 +1073,18 @@
         <v>1.33</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1097,7 +1097,7 @@
         <v>0.13</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1105,10 +1105,10 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1129,10 +1129,10 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1153,10 +1153,10 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1174,10 +1174,10 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1195,10 +1195,10 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -1213,13 +1213,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
         <v>87</v>
-      </c>
-      <c r="B24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" t="s">
-        <v>89</v>
       </c>
       <c r="D24">
         <v>1</v>

</xml_diff>